<commit_message>
Promoted @deepas design as top level for submission process. Updated testbench as per new design.
</commit_message>
<xml_diff>
--- a/rtl/MS1/dnn.xlsx
+++ b/rtl/MS1/dnn.xlsx
@@ -5,15 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit\Box\Sumit-PhD\ECE755\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit\Box\Sumit-PhD\ECE755\Project\DNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E58A5DC-44D0-4D41-B128-6D546C4F383E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC92D404-A164-4F13-8A0B-7AC75CBE61F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Few Negative" sheetId="1" r:id="rId1"/>
+    <sheet name="All Positive" sheetId="2" r:id="rId2"/>
+    <sheet name="minimum" sheetId="3" r:id="rId3"/>
+    <sheet name="maximum" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="35">
   <si>
     <t>x0</t>
   </si>
@@ -136,6 +139,9 @@
   </si>
   <si>
     <t>w37</t>
+  </si>
+  <si>
+    <t>After ReLu</t>
   </si>
 </sst>
 </file>
@@ -453,15 +459,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M26"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>26</v>
       </c>
@@ -475,13 +486,325 @@
         <v>29</v>
       </c>
       <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
         <v>30</v>
       </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>B3*B8+B4*B9+B5*B10+B6*B11</f>
+        <v>62</v>
+      </c>
+      <c r="H3">
+        <f>B3*B13+B4*B14+B5*B15+B6*B16</f>
+        <v>-36</v>
+      </c>
+      <c r="I3">
+        <f>B3*B18+B4*B19+B5*B20+B6*B21</f>
+        <v>-21</v>
+      </c>
+      <c r="J3">
+        <f>B3*B23+B4*B24+B5*B25+B6*B26</f>
+        <v>66</v>
+      </c>
+      <c r="L3">
+        <f>MAX(G3,0)</f>
+        <v>62</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:O3" si="0">MAX(H3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="Q3">
+        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
+        <v>-726</v>
+      </c>
+      <c r="R3">
+        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
+        <v>-348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>-6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB765798-F849-44B5-BAE4-6735C85FA5EE}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
       <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -511,15 +834,31 @@
         <v>96</v>
       </c>
       <c r="L3">
-        <f>E3*G3+E4*H3+E5*I3+E6*J3</f>
+        <f>MAX(G3, 0)</f>
+        <v>68</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:O3" si="0">MAX(H3, 0)</f>
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="Q3">
+        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
         <v>1173</v>
       </c>
-      <c r="M3">
-        <f>E8*G3+E9*H3+E10*I3+E11*J3</f>
+      <c r="R3">
+        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
         <v>1392</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -533,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -547,7 +886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -561,7 +900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -575,7 +914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -589,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -603,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -617,7 +956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -625,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -633,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -641,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -649,7 +988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -657,7 +996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -665,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -673,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -681,7 +1020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -689,7 +1028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -697,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -705,12 +1044,612 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
       <c r="B26">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A8C105-FF61-4FCA-B0C7-DD5CF022DEB1}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>-16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>-16</v>
+      </c>
+      <c r="G3">
+        <f>B3*B8+B4*B9+B5*B10+B6*B11</f>
+        <v>1024</v>
+      </c>
+      <c r="H3">
+        <f>B3*B13+B4*B14+B5*B15+B6*B16</f>
+        <v>1024</v>
+      </c>
+      <c r="I3">
+        <f>B3*B18+B4*B19+B5*B20+B6*B21</f>
+        <v>1024</v>
+      </c>
+      <c r="J3">
+        <f>B3*B23+B4*B24+B5*B25+B6*B26</f>
+        <v>1024</v>
+      </c>
+      <c r="L3">
+        <f>MAX(G3,0)</f>
+        <v>1024</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:O3" si="0">MAX(H3,0)</f>
+        <v>1024</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="Q3">
+        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
+        <v>-65536</v>
+      </c>
+      <c r="R3">
+        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
+        <v>-65536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>-16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>-16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>-16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>-16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>-16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>-16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>-16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>-16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD24435-2B40-44E0-816F-2FDFD9D58F2D}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <f>B3*B8+B4*B9+B5*B10+B6*B11</f>
+        <v>900</v>
+      </c>
+      <c r="H3">
+        <f>B3*B13+B4*B14+B5*B15+B6*B16</f>
+        <v>900</v>
+      </c>
+      <c r="I3">
+        <f>B3*B18+B4*B19+B5*B20+B6*B21</f>
+        <v>900</v>
+      </c>
+      <c r="J3">
+        <f>B3*B23+B4*B24+B5*B25+B6*B26</f>
+        <v>900</v>
+      </c>
+      <c r="L3">
+        <f>MAX(G3,0)</f>
+        <v>900</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:O3" si="0">MAX(H3,0)</f>
+        <v>900</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="Q3">
+        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
+        <v>54000</v>
+      </c>
+      <c r="R3">
+        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testbench to perform 3 more tests, and verified design. Increased middle layers bit by 1 (11 bits -> 12 bits) to account for signed bit. Updated .gitignore to not include vsim build files
</commit_message>
<xml_diff>
--- a/rtl/MS1/dnn.xlsx
+++ b/rtl/MS1/dnn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumit\Box\Sumit-PhD\ECE755\Project\DNN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwprod-my.sharepoint.com/personal/belatikar_wisc_edu/Documents/Spring'22/ECE755/Project/gnn-accelerator/rtl/ms1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC92D404-A164-4F13-8A0B-7AC75CBE61F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{FC92D404-A164-4F13-8A0B-7AC75CBE61F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C780E6B-17D6-4B6C-82E9-DA6BC5BDB3C5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1344" yWindow="384" windowWidth="16560" windowHeight="9420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Few Negative" sheetId="1" r:id="rId1"/>
@@ -461,18 +461,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>26</v>
       </c>
@@ -504,7 +504,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -558,7 +558,7 @@
         <v>-348</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -572,7 +572,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -586,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -600,7 +600,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -614,7 +614,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -628,7 +628,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -642,7 +642,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -656,7 +656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -664,7 +664,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -672,7 +672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -680,7 +680,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -688,7 +688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -696,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -704,7 +704,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -712,7 +712,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -720,7 +720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -728,7 +728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -736,7 +736,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -744,7 +744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -759,20 +759,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB765798-F849-44B5-BAE4-6735C85FA5EE}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="Q3" sqref="Q3:R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>26</v>
       </c>
@@ -804,33 +804,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="G3">
-        <f>B3*B8+B4*B9+B5*B10+B6*B11</f>
+        <f>B3*B7+B4*B8+B5*B9+B6*B10</f>
         <v>68</v>
       </c>
       <c r="H3">
-        <f>B3*B13+B4*B14+B5*B15+B6*B16</f>
+        <f>B3*B11+B4*B12+B5*B13+B6*B14</f>
         <v>14</v>
       </c>
       <c r="I3">
-        <f>B3*B18+B4*B19+B5*B20+B6*B21</f>
+        <f>B3*B15+B4*B16+B5*B17+B6*B18</f>
         <v>39</v>
       </c>
       <c r="J3">
-        <f>B3*B23+B4*B24+B5*B25+B6*B26</f>
+        <f>B3*B19+B4*B20+B5*B21+B6*B22</f>
         <v>96</v>
       </c>
       <c r="L3">
@@ -850,206 +844,228 @@
         <v>96</v>
       </c>
       <c r="Q3">
-        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
+        <f>B23*L3+B24*M3+B25*N3+B26*O3</f>
         <v>1173</v>
       </c>
       <c r="R3">
-        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
+        <f>B27*L3+B28*M3+B29*N3+B30*O3</f>
         <v>1392</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
         <v>9</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28">
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1059,20 +1075,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A8C105-FF61-4FCA-B0C7-DD5CF022DEB1}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>26</v>
       </c>
@@ -1104,33 +1120,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>-16</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>-16</v>
-      </c>
       <c r="G3">
-        <f>B3*B8+B4*B9+B5*B10+B6*B11</f>
+        <f>B3*B7+B4*B8+B5*B9+B6*B10</f>
         <v>1024</v>
       </c>
       <c r="H3">
-        <f>B3*B13+B4*B14+B5*B15+B6*B16</f>
+        <f>B3*B11+B4*B12+B5*B13+B6*B14</f>
         <v>1024</v>
       </c>
       <c r="I3">
-        <f>B3*B18+B4*B19+B5*B20+B6*B21</f>
+        <f>B3*B15+B4*B16+B5*B17+B6*B18</f>
         <v>1024</v>
       </c>
       <c r="J3">
-        <f>B3*B23+B4*B24+B5*B25+B6*B26</f>
+        <f>B3*B19+B4*B20+B5*B21+B6*B22</f>
         <v>1024</v>
       </c>
       <c r="L3">
@@ -1150,205 +1160,227 @@
         <v>1024</v>
       </c>
       <c r="Q3">
-        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
+        <f>B23*L3+B24*M3+B25*N3+B26*O3</f>
         <v>-65536</v>
       </c>
       <c r="R3">
-        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
+        <f>B27*L3+B28*M3+B29*N3+B30*O3</f>
         <v>-65536</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>-16</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>-16</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>-16</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>-16</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B26">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>-16</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B27">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="E9">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>-16</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B28">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="E10">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>-16</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B29">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="E11">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26">
+      <c r="B30">
         <v>-16</v>
       </c>
     </row>
@@ -1359,20 +1391,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD24435-2B40-44E0-816F-2FDFD9D58F2D}">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>26</v>
       </c>
@@ -1404,17 +1436,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
         <v>15</v>
       </c>
       <c r="G3">
@@ -1422,15 +1448,15 @@
         <v>900</v>
       </c>
       <c r="H3">
-        <f>B3*B13+B4*B14+B5*B15+B6*B16</f>
+        <f>B3*B12+B4*B13+B5*B14+B6*B15</f>
         <v>900</v>
       </c>
       <c r="I3">
-        <f>B3*B18+B4*B19+B5*B20+B6*B21</f>
+        <f>B3*B16+B4*B17+B5*B18+B6*B19</f>
         <v>900</v>
       </c>
       <c r="J3">
-        <f>B3*B23+B4*B24+B5*B25+B6*B26</f>
+        <f>B3*B20+B4*B21+B5*B22+B6*B23</f>
         <v>900</v>
       </c>
       <c r="L3">
@@ -1450,205 +1476,227 @@
         <v>900</v>
       </c>
       <c r="Q3">
-        <f>E3*L3+E4*M3+E5*N3+E6*O3</f>
+        <f>B24*L3+B25*M3+B26*N3+B27*O3</f>
         <v>54000</v>
       </c>
       <c r="R3">
-        <f>E8*L3+E9*M3+E10*N3+E11*O3</f>
+        <f>B28*L3+B29*M3+B30*N3+B31*O3</f>
         <v>54000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>25</v>
       </c>
-      <c r="E11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26">
+      <c r="B31">
         <v>15</v>
       </c>
     </row>

</xml_diff>